<commit_message>
增加 project builder ； builder 存在 bug ，下一步解决；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24AFD4B-F2A4-453C-B869-A7E281E7B3CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE31249-F0A8-46E2-8488-E0C9438F1875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,14 @@
   </si>
   <si>
     <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每当玩家升级地产时，获得500元。当任意玩家到建筑公司时，可将一处地产升一级（需支付升级费用）。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,11 +477,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -728,39 +736,24 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>300</v>
-      </c>
-      <c r="E8" s="1">
-        <v>600</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1500</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3500</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="I8" s="1">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="J8" s="1">
-        <v>700</v>
-      </c>
-      <c r="K8" s="1">
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -768,7 +761,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -777,7 +770,7 @@
         <v>300</v>
       </c>
       <c r="E9" s="1">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F9" s="1">
         <v>1500</v>
@@ -786,13 +779,13 @@
         <v>3500</v>
       </c>
       <c r="H9" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="I9" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="J9" s="1">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="K9" s="1">
         <v>300</v>
@@ -803,34 +796,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E10" s="1">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F10" s="1">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="G10" s="1">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="H10" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I10" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="J10" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="K10" s="1">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -838,7 +831,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -847,22 +840,22 @@
         <v>400</v>
       </c>
       <c r="E11" s="1">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="F11" s="1">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="G11" s="1">
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="H11" s="1">
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="I11" s="1">
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="J11" s="1">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="K11" s="1">
         <v>600</v>
@@ -873,31 +866,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
         <v>400</v>
       </c>
       <c r="E12" s="1">
+        <v>900</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J12" s="1">
         <v>1000</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G12" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H12" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1100</v>
       </c>
       <c r="K12" s="1">
         <v>600</v>
@@ -908,34 +901,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E13" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="F13" s="1">
-        <v>4500</v>
+        <v>2500</v>
       </c>
       <c r="G13" s="1">
-        <v>9000</v>
+        <v>5500</v>
       </c>
       <c r="H13" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="I13" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="J13" s="1">
-        <v>1900</v>
+        <v>1100</v>
       </c>
       <c r="K13" s="1">
-        <v>900</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -943,7 +936,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -952,22 +945,22 @@
         <v>700</v>
       </c>
       <c r="E14" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F14" s="1">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="G14" s="1">
-        <v>8500</v>
+        <v>9000</v>
       </c>
       <c r="H14" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="I14" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="J14" s="1">
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="K14" s="1">
         <v>900</v>
@@ -978,34 +971,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E15" s="1">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="F15" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="G15" s="1">
-        <v>10500</v>
+        <v>8500</v>
       </c>
       <c r="H15" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="I15" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J15" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="K15" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1013,7 +1006,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -1040,6 +1033,41 @@
         <v>2000</v>
       </c>
       <c r="K16" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>800</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G17" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K17" s="1">
         <v>1200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 project builder 功能；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE31249-F0A8-46E2-8488-E0C9438F1875}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDCABE3-804C-4C00-B939-3D10CD7F4FA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,14 @@
   </si>
   <si>
     <t>每当玩家升级地产时，获得500元。当任意玩家到建筑公司时，可将一处地产升一级（需支付升级费用）。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大陆运输</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当你拥有1/2/3项运输项目时，收取500/1000/2000元。下回合开始时，你可以放弃投骰子，改为给本项目拥有着500元（无人拥有则给银行），立即到任意一个地产处。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -477,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -861,39 +869,24 @@
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>400</v>
-      </c>
-      <c r="E12" s="1">
-        <v>900</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G12" s="1">
-        <v>5000</v>
+        <v>31</v>
       </c>
       <c r="H12" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I12" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K12" s="1">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -901,31 +894,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1">
         <v>400</v>
       </c>
       <c r="E13" s="1">
+        <v>900</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J13" s="1">
         <v>1000</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G13" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1100</v>
       </c>
       <c r="K13" s="1">
         <v>600</v>
@@ -936,34 +929,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E14" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="1">
-        <v>4500</v>
+        <v>2500</v>
       </c>
       <c r="G14" s="1">
-        <v>9000</v>
+        <v>5500</v>
       </c>
       <c r="H14" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="I14" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="J14" s="1">
-        <v>1900</v>
+        <v>1100</v>
       </c>
       <c r="K14" s="1">
-        <v>900</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -971,7 +964,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -980,22 +973,22 @@
         <v>700</v>
       </c>
       <c r="E15" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F15" s="1">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="G15" s="1">
-        <v>8500</v>
+        <v>9000</v>
       </c>
       <c r="H15" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="I15" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="J15" s="1">
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="K15" s="1">
         <v>900</v>
@@ -1006,34 +999,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E16" s="1">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="F16" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="G16" s="1">
-        <v>10500</v>
+        <v>8500</v>
       </c>
       <c r="H16" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="I16" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J16" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="K16" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1041,7 +1034,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1068,6 +1061,41 @@
         <v>2000</v>
       </c>
       <c r="K17" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>800</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="K18" s="1">
         <v>1200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
去掉 #type: ignore 标识符；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8FF703-D2E9-44BA-A325-20BAD9282F91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D607A895-4B8D-415B-A9BA-E7003011590D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21090" yWindow="720" windowWidth="13785" windowHeight="8430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -203,6 +203,14 @@
   </si>
   <si>
     <t>钓鱼岛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>起点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过时领取奖励4000元，若刚好到达起点，可将自己任意一处地产升一级（仍需支付升级费用）。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -537,11 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -601,39 +609,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>400</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G2" s="3">
-        <v>5500</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2400</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2400</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1200</v>
-      </c>
-      <c r="K2" s="1">
-        <v>600</v>
+        <v>46</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -641,89 +625,89 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E3" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G3" s="1">
-        <v>6000</v>
+        <v>2500</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5500</v>
       </c>
       <c r="H3" s="1">
-        <v>2600</v>
+        <v>2400</v>
       </c>
       <c r="I3" s="1">
-        <v>2600</v>
+        <v>2400</v>
       </c>
       <c r="J3" s="1">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="K3" s="1">
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1100</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6000</v>
       </c>
       <c r="H4" s="1">
-        <v>3500</v>
+        <v>2600</v>
       </c>
       <c r="I4" s="1">
-        <v>3000</v>
+        <v>2600</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1300</v>
+      </c>
+      <c r="K4" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>400</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G5" s="1">
-        <v>5500</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1">
-        <v>2300</v>
+        <v>3500</v>
       </c>
       <c r="I5" s="1">
-        <v>2300</v>
+        <v>3000</v>
       </c>
       <c r="J5" s="1">
-        <v>1100</v>
-      </c>
-      <c r="K5" s="1">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -731,34 +715,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E6" s="1">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="1">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="G6" s="1">
-        <v>3000</v>
+        <v>5500</v>
       </c>
       <c r="H6" s="1">
-        <v>1200</v>
+        <v>2300</v>
       </c>
       <c r="I6" s="1">
-        <v>1200</v>
+        <v>2300</v>
       </c>
       <c r="J6" s="1">
+        <v>1100</v>
+      </c>
+      <c r="K6" s="1">
         <v>600</v>
-      </c>
-      <c r="K6" s="1">
-        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -766,89 +750,89 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>200</v>
       </c>
       <c r="E7" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="F7" s="1">
         <v>1000</v>
       </c>
       <c r="G7" s="1">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="H7" s="1">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="I7" s="1">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="J7" s="1">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="K7" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1">
+        <v>400</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2500</v>
       </c>
       <c r="H8" s="1">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="I8" s="1">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="K8" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>300</v>
-      </c>
-      <c r="E9" s="1">
-        <v>600</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1500</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3500</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="I9" s="1">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="J9" s="1">
-        <v>700</v>
-      </c>
-      <c r="K9" s="1">
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -856,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -865,7 +849,7 @@
         <v>300</v>
       </c>
       <c r="E10" s="1">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F10" s="1">
         <v>1500</v>
@@ -874,13 +858,13 @@
         <v>3500</v>
       </c>
       <c r="H10" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="I10" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="J10" s="1">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="K10" s="1">
         <v>300</v>
@@ -891,89 +875,89 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E11" s="1">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F11" s="1">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="G11" s="1">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="H11" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I11" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="J11" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="K11" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>400</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5500</v>
       </c>
       <c r="H12" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="I12" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="K12" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>400</v>
-      </c>
-      <c r="E13" s="1">
-        <v>900</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G13" s="1">
-        <v>5000</v>
+        <v>31</v>
       </c>
       <c r="H13" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I13" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K13" s="1">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -981,31 +965,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>400</v>
       </c>
       <c r="E14" s="1">
+        <v>900</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J14" s="1">
         <v>1000</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G14" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H14" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I14" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1100</v>
       </c>
       <c r="K14" s="1">
         <v>600</v>
@@ -1016,34 +1000,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E15" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="F15" s="1">
-        <v>4500</v>
+        <v>2500</v>
       </c>
       <c r="G15" s="1">
-        <v>9000</v>
+        <v>5500</v>
       </c>
       <c r="H15" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="I15" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="J15" s="1">
-        <v>1900</v>
+        <v>1100</v>
       </c>
       <c r="K15" s="1">
-        <v>900</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1051,7 +1035,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -1060,22 +1044,22 @@
         <v>700</v>
       </c>
       <c r="E16" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F16" s="1">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="G16" s="1">
-        <v>8500</v>
+        <v>9000</v>
       </c>
       <c r="H16" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="I16" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="J16" s="1">
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="K16" s="1">
         <v>900</v>
@@ -1086,34 +1070,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E17" s="1">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="F17" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="G17" s="1">
-        <v>10500</v>
+        <v>8500</v>
       </c>
       <c r="H17" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="I17" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J17" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="K17" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1121,7 +1105,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -1151,47 +1135,47 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>800</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10500</v>
       </c>
       <c r="H19" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I19" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
-        <v>600</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3500</v>
-      </c>
-      <c r="G20" s="1">
-        <v>7500</v>
+        <v>33</v>
       </c>
       <c r="H20" s="1">
         <v>3000</v>
@@ -1200,10 +1184,10 @@
         <v>3000</v>
       </c>
       <c r="J20" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K20" s="1">
-        <v>900</v>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1211,7 +1195,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -1220,22 +1204,22 @@
         <v>600</v>
       </c>
       <c r="E21" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G21" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J21" s="1">
         <v>1500</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G21" s="1">
-        <v>8500</v>
-      </c>
-      <c r="H21" s="1">
-        <v>3300</v>
-      </c>
-      <c r="I21" s="1">
-        <v>3300</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1600</v>
       </c>
       <c r="K21" s="1">
         <v>900</v>
@@ -1246,89 +1230,89 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>600</v>
       </c>
       <c r="E22" s="1">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F22" s="1">
         <v>4000</v>
       </c>
       <c r="G22" s="1">
-        <v>8000</v>
+        <v>8500</v>
       </c>
       <c r="H22" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="I22" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="J22" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="K22" s="1">
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>600</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G23" s="1">
+        <v>8000</v>
       </c>
       <c r="H23" s="1">
-        <v>3500</v>
+        <v>3100</v>
       </c>
       <c r="I23" s="1">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K23" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="1">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>800</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F24" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G24" s="1">
-        <v>11000</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="I24" s="1">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="J24" s="1">
-        <v>2200</v>
-      </c>
-      <c r="K24" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1336,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -1366,59 +1350,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>800</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F26" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G26" s="1">
+        <v>11000</v>
       </c>
       <c r="H26" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="I26" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="J26" s="1">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2200</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="1">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1">
-        <v>900</v>
-      </c>
-      <c r="E27" s="1">
-        <v>2100</v>
-      </c>
-      <c r="F27" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G27" s="1">
-        <v>12000</v>
+        <v>41</v>
       </c>
       <c r="H27" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="I27" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="J27" s="1">
-        <v>2400</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1426,34 +1410,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
         <v>6</v>
       </c>
       <c r="D28" s="1">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E28" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G28" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I28" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J28" s="1">
         <v>2400</v>
       </c>
-      <c r="F28" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G28" s="1">
-        <v>13000</v>
-      </c>
-      <c r="H28" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I28" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J28" s="1">
-        <v>2500</v>
-      </c>
       <c r="K28" s="1">
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1461,7 +1445,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1">
         <v>6</v>
@@ -1473,16 +1457,16 @@
         <v>2400</v>
       </c>
       <c r="F29" s="1">
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="G29" s="1">
-        <v>13500</v>
+        <v>13000</v>
       </c>
       <c r="H29" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="I29" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="J29" s="1">
         <v>2500</v>
@@ -1496,33 +1480,68 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1">
         <v>6</v>
       </c>
       <c r="D30" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="1">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="F30" s="1">
         <v>6500</v>
       </c>
       <c r="G30" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H30" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I30" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F31" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G31" s="1">
         <v>14000</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H31" s="1">
         <v>5500</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I31" s="1">
         <v>5500</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J31" s="1">
         <v>2700</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K31" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 project tv 功能；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D607A895-4B8D-415B-A9BA-E7003011590D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDEEF3D-6B25-4555-9322-2C139AD59229}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>event</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>沈阳</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,6 +207,30 @@
   </si>
   <si>
     <t>经过时领取奖励4000元，若刚好到达起点，可将自己任意一处地产升一级（仍需支付升级费用）。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>public</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽取1张新闻卡。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新闻2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新闻1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电视台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当任何人走到运气和新闻时，你获得500元奖励。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,11 +565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -570,31 +590,31 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -606,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
@@ -614,10 +634,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -625,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -660,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -695,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="1">
         <v>3500</v>
@@ -707,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -715,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -750,34 +770,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>200</v>
-      </c>
-      <c r="E7" s="1">
-        <v>500</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="J7" s="1">
-        <v>600</v>
-      </c>
-      <c r="K7" s="1">
-        <v>300</v>
+        <v>50</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -785,89 +781,89 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>200</v>
       </c>
       <c r="E8" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="F8" s="1">
         <v>1000</v>
       </c>
       <c r="G8" s="1">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="H8" s="1">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="I8" s="1">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="J8" s="1">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="K8" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>200</v>
+      </c>
+      <c r="E9" s="1">
+        <v>400</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2500</v>
       </c>
       <c r="H9" s="1">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="I9" s="1">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="K9" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>300</v>
-      </c>
-      <c r="E10" s="1">
-        <v>600</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1500</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3500</v>
+        <v>28</v>
       </c>
       <c r="H10" s="1">
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="I10" s="1">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="J10" s="1">
-        <v>700</v>
-      </c>
-      <c r="K10" s="1">
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -875,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -884,7 +880,7 @@
         <v>300</v>
       </c>
       <c r="E11" s="1">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F11" s="1">
         <v>1500</v>
@@ -893,13 +889,13 @@
         <v>3500</v>
       </c>
       <c r="H11" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="I11" s="1">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="J11" s="1">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="K11" s="1">
         <v>300</v>
@@ -910,89 +906,89 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E12" s="1">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F12" s="1">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="G12" s="1">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="H12" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I12" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="J12" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="K12" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>400</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5500</v>
       </c>
       <c r="H13" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="I13" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="K13" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>400</v>
-      </c>
-      <c r="E14" s="1">
-        <v>900</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G14" s="1">
-        <v>5000</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I14" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J14" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K14" s="1">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1000,31 +996,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>400</v>
       </c>
       <c r="E15" s="1">
+        <v>900</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J15" s="1">
         <v>1000</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G15" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H15" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I15" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1100</v>
       </c>
       <c r="K15" s="1">
         <v>600</v>
@@ -1035,365 +1031,341 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="E16" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="F16" s="1">
-        <v>4500</v>
+        <v>2500</v>
       </c>
       <c r="G16" s="1">
-        <v>9000</v>
+        <v>5500</v>
       </c>
       <c r="H16" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="I16" s="1">
-        <v>3800</v>
+        <v>2200</v>
       </c>
       <c r="J16" s="1">
-        <v>1900</v>
+        <v>1100</v>
       </c>
       <c r="K16" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>700</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1500</v>
-      </c>
-      <c r="F17" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G17" s="1">
-        <v>8500</v>
+        <v>51</v>
       </c>
       <c r="H17" s="1">
         <v>3500</v>
       </c>
       <c r="I17" s="1">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="J17" s="1">
-        <v>1700</v>
-      </c>
-      <c r="K17" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E18" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4500</v>
+      </c>
+      <c r="G18" s="1">
+        <v>9000</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3800</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3800</v>
+      </c>
+      <c r="J18" s="1">
         <v>1900</v>
       </c>
-      <c r="F18" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G18" s="1">
-        <v>10500</v>
-      </c>
-      <c r="H18" s="1">
-        <v>4000</v>
-      </c>
-      <c r="I18" s="1">
-        <v>4000</v>
-      </c>
-      <c r="J18" s="1">
-        <v>2000</v>
-      </c>
       <c r="K18" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E19" s="1">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="F19" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="G19" s="1">
-        <v>10500</v>
+        <v>8500</v>
       </c>
       <c r="H19" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="I19" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J19" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="K19" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>800</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G20" s="1">
+        <v>10500</v>
       </c>
       <c r="H20" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I20" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="E21" s="1">
-        <v>1400</v>
+        <v>1900</v>
       </c>
       <c r="F21" s="1">
-        <v>3500</v>
+        <v>5000</v>
       </c>
       <c r="G21" s="1">
-        <v>7500</v>
+        <v>10500</v>
       </c>
       <c r="H21" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I21" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J21" s="1">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K21" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="1">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1">
-        <v>600</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1500</v>
-      </c>
-      <c r="F22" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G22" s="1">
-        <v>8500</v>
+        <v>32</v>
       </c>
       <c r="H22" s="1">
-        <v>3300</v>
+        <v>3000</v>
       </c>
       <c r="I22" s="1">
-        <v>3300</v>
+        <v>3000</v>
       </c>
       <c r="J22" s="1">
-        <v>1600</v>
-      </c>
-      <c r="K22" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1">
-        <v>600</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F23" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G23" s="1">
-        <v>8000</v>
-      </c>
-      <c r="H23" s="1">
-        <v>3100</v>
-      </c>
-      <c r="I23" s="1">
-        <v>3100</v>
-      </c>
-      <c r="J23" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K23" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>600</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7500</v>
       </c>
       <c r="H24" s="1">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="I24" s="1">
         <v>3000</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K24" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E25" s="1">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="F25" s="1">
-        <v>5500</v>
+        <v>4000</v>
       </c>
       <c r="G25" s="1">
-        <v>11000</v>
+        <v>8500</v>
       </c>
       <c r="H25" s="1">
-        <v>4400</v>
+        <v>3300</v>
       </c>
       <c r="I25" s="1">
-        <v>4400</v>
+        <v>3300</v>
       </c>
       <c r="J25" s="1">
-        <v>2200</v>
+        <v>1600</v>
       </c>
       <c r="K25" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1">
         <v>5</v>
       </c>
       <c r="D26" s="1">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E26" s="1">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="F26" s="1">
-        <v>5500</v>
+        <v>4000</v>
       </c>
       <c r="G26" s="1">
-        <v>11000</v>
+        <v>8000</v>
       </c>
       <c r="H26" s="1">
-        <v>4400</v>
+        <v>3100</v>
       </c>
       <c r="I26" s="1">
-        <v>4400</v>
+        <v>3100</v>
       </c>
       <c r="J26" s="1">
-        <v>2200</v>
+        <v>1500</v>
       </c>
       <c r="K26" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="71.25" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H27" s="1">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="I27" s="1">
         <v>3000</v>
@@ -1402,146 +1374,236 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="E28" s="1">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="F28" s="1">
         <v>5500</v>
       </c>
       <c r="G28" s="1">
-        <v>12000</v>
+        <v>11000</v>
       </c>
       <c r="H28" s="1">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="I28" s="1">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="J28" s="1">
-        <v>2400</v>
+        <v>2200</v>
       </c>
       <c r="K28" s="1">
         <v>1200</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="E29" s="1">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="F29" s="1">
-        <v>6000</v>
+        <v>5500</v>
       </c>
       <c r="G29" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="H29" s="1">
-        <v>5000</v>
+        <v>4400</v>
       </c>
       <c r="I29" s="1">
-        <v>5000</v>
+        <v>4400</v>
       </c>
       <c r="J29" s="1">
-        <v>2500</v>
+        <v>2200</v>
       </c>
       <c r="K29" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="1">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F30" s="1">
-        <v>6500</v>
-      </c>
-      <c r="G30" s="1">
-        <v>13500</v>
+        <v>40</v>
       </c>
       <c r="H30" s="1">
-        <v>5100</v>
+        <v>3000</v>
       </c>
       <c r="I30" s="1">
-        <v>5100</v>
+        <v>3000</v>
       </c>
       <c r="J30" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K30" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1">
         <v>6</v>
       </c>
       <c r="D31" s="1">
+        <v>900</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G31" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I31" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2400</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6000</v>
+      </c>
+      <c r="G32" s="1">
+        <v>13000</v>
+      </c>
+      <c r="H32" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I32" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F33" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G33" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I33" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1">
         <v>1100</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E34" s="1">
         <v>2500</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F34" s="1">
         <v>6500</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G34" s="1">
         <v>14000</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H34" s="1">
         <v>5500</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I34" s="1">
         <v>5500</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J34" s="1">
         <v>2700</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K34" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
增加 public luck ； 修复 logging bug；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDEEF3D-6B25-4555-9322-2C139AD59229}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D90B1-B763-4BD5-B711-CBA8CAB0849A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -231,6 +231,18 @@
   </si>
   <si>
     <t>当任何人走到运气和新闻时，你获得500元奖励。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运气1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽取1张运气卡。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运气2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,11 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1031,89 +1043,65 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>400</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G16" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1100</v>
-      </c>
-      <c r="K16" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>400</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5500</v>
       </c>
       <c r="H17" s="1">
-        <v>3500</v>
+        <v>2200</v>
       </c>
       <c r="I17" s="1">
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+      <c r="K17" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>700</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1600</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4500</v>
-      </c>
-      <c r="G18" s="1">
-        <v>9000</v>
+        <v>51</v>
       </c>
       <c r="H18" s="1">
-        <v>3800</v>
+        <v>3500</v>
       </c>
       <c r="I18" s="1">
-        <v>3800</v>
+        <v>3000</v>
       </c>
       <c r="J18" s="1">
-        <v>1900</v>
-      </c>
-      <c r="K18" s="1">
-        <v>900</v>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1121,7 +1109,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -1130,22 +1118,22 @@
         <v>700</v>
       </c>
       <c r="E19" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F19" s="1">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="G19" s="1">
-        <v>8500</v>
+        <v>9000</v>
       </c>
       <c r="H19" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="I19" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="J19" s="1">
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="K19" s="1">
         <v>900</v>
@@ -1156,34 +1144,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="E20" s="1">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="F20" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="G20" s="1">
-        <v>10500</v>
+        <v>8500</v>
       </c>
       <c r="H20" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="I20" s="1">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="J20" s="1">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="K20" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1191,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -1221,35 +1209,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>800</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F22" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G22" s="1">
+        <v>10500</v>
       </c>
       <c r="H22" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I22" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1257,34 +1269,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4</v>
-      </c>
-      <c r="D24" s="1">
-        <v>600</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F24" s="1">
-        <v>3500</v>
-      </c>
-      <c r="G24" s="1">
-        <v>7500</v>
-      </c>
-      <c r="H24" s="1">
-        <v>3000</v>
-      </c>
-      <c r="I24" s="1">
-        <v>3000</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K24" s="1">
-        <v>900</v>
+        <v>49</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1292,7 +1280,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -1301,22 +1289,22 @@
         <v>600</v>
       </c>
       <c r="E25" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G25" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J25" s="1">
         <v>1500</v>
-      </c>
-      <c r="F25" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G25" s="1">
-        <v>8500</v>
-      </c>
-      <c r="H25" s="1">
-        <v>3300</v>
-      </c>
-      <c r="I25" s="1">
-        <v>3300</v>
-      </c>
-      <c r="J25" s="1">
-        <v>1600</v>
       </c>
       <c r="K25" s="1">
         <v>900</v>
@@ -1327,89 +1315,89 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>600</v>
       </c>
       <c r="E26" s="1">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F26" s="1">
         <v>4000</v>
       </c>
       <c r="G26" s="1">
-        <v>8000</v>
+        <v>8500</v>
       </c>
       <c r="H26" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="I26" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="J26" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="K26" s="1">
         <v>900</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>600</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G27" s="1">
+        <v>8000</v>
       </c>
       <c r="H27" s="1">
-        <v>3500</v>
+        <v>3100</v>
       </c>
       <c r="I27" s="1">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K27" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="1">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1">
-        <v>800</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F28" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G28" s="1">
-        <v>11000</v>
+        <v>36</v>
       </c>
       <c r="H28" s="1">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="I28" s="1">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="J28" s="1">
-        <v>2200</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1417,7 +1405,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1">
         <v>5</v>
@@ -1447,59 +1435,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>800</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G30" s="1">
+        <v>11000</v>
       </c>
       <c r="H30" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="I30" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="J30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2200</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1">
-        <v>900</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2100</v>
-      </c>
-      <c r="F31" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G31" s="1">
-        <v>12000</v>
+        <v>40</v>
       </c>
       <c r="H31" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="I31" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="J31" s="1">
-        <v>2400</v>
-      </c>
-      <c r="K31" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1507,103 +1495,149 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1">
         <v>6</v>
       </c>
       <c r="D32" s="1">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E32" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G32" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H32" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I32" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J32" s="1">
         <v>2400</v>
       </c>
-      <c r="F32" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G32" s="1">
-        <v>13000</v>
-      </c>
-      <c r="H32" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I32" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J32" s="1">
-        <v>2500</v>
-      </c>
       <c r="K32" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="1">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F33" s="1">
-        <v>6500</v>
-      </c>
-      <c r="G33" s="1">
-        <v>13500</v>
-      </c>
-      <c r="H33" s="1">
-        <v>5100</v>
-      </c>
-      <c r="I33" s="1">
-        <v>5100</v>
-      </c>
-      <c r="J33" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K33" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34" s="1">
         <v>6</v>
       </c>
       <c r="D34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6000</v>
+      </c>
+      <c r="G34" s="1">
+        <v>13000</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I34" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="1">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F35" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G35" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H35" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I35" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J35" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
         <v>1100</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E36" s="1">
         <v>2500</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F36" s="1">
         <v>6500</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G36" s="1">
         <v>14000</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H36" s="1">
         <v>5500</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I36" s="1">
         <v>5500</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J36" s="1">
         <v>2700</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K36" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 public park 功能；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300D90B1-B763-4BD5-B711-CBA8CAB0849A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E15724-5735-4972-93CC-F867DD2F359F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,6 +243,14 @@
   </si>
   <si>
     <t>运气2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公园</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拾到300元。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,11 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1350,89 +1358,65 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="1">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1">
-        <v>600</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F27" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G27" s="1">
-        <v>8000</v>
-      </c>
-      <c r="H27" s="1">
-        <v>3100</v>
-      </c>
-      <c r="I27" s="1">
-        <v>3100</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K27" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>600</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G28" s="1">
+        <v>8000</v>
       </c>
       <c r="H28" s="1">
-        <v>3500</v>
+        <v>3100</v>
       </c>
       <c r="I28" s="1">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="J28" s="1">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K28" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1">
-        <v>5</v>
-      </c>
-      <c r="D29" s="1">
-        <v>800</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F29" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G29" s="1">
-        <v>11000</v>
+        <v>36</v>
       </c>
       <c r="H29" s="1">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="I29" s="1">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="J29" s="1">
-        <v>2200</v>
-      </c>
-      <c r="K29" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -1440,7 +1424,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1">
         <v>5</v>
@@ -1470,59 +1454,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>800</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G31" s="1">
+        <v>11000</v>
       </c>
       <c r="H31" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="I31" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="J31" s="1">
-        <v>0</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2200</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1">
-        <v>900</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2100</v>
-      </c>
-      <c r="F32" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G32" s="1">
-        <v>12000</v>
+        <v>40</v>
       </c>
       <c r="H32" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="I32" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="J32" s="1">
-        <v>2400</v>
-      </c>
-      <c r="K32" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -1530,10 +1514,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>900</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F33" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G33" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H33" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I33" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2400</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -1541,34 +1549,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="1">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E34" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F34" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G34" s="1">
-        <v>13000</v>
-      </c>
-      <c r="H34" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I34" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J34" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K34" s="1">
-        <v>1500</v>
+        <v>55</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -1576,7 +1560,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
@@ -1588,16 +1572,16 @@
         <v>2400</v>
       </c>
       <c r="F35" s="1">
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="G35" s="1">
-        <v>13500</v>
+        <v>13000</v>
       </c>
       <c r="H35" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="I35" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="J35" s="1">
         <v>2500</v>
@@ -1611,33 +1595,68 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
       </c>
       <c r="D36" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E36" s="1">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="F36" s="1">
         <v>6500</v>
       </c>
       <c r="G36" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H36" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I36" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F37" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G37" s="1">
         <v>14000</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H37" s="1">
         <v>5500</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I37" s="1">
         <v>5500</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J37" s="1">
         <v>2700</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K37" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 public tax ；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E15724-5735-4972-93CC-F867DD2F359F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C50BE2B-19C0-4D17-80C6-032227159185}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,6 +251,14 @@
   </si>
   <si>
     <t>拾到300元。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>税务中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缴纳每块地产300元税金。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,11 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1595,34 +1603,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="1">
-        <v>6</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E36" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F36" s="1">
-        <v>6500</v>
-      </c>
-      <c r="G36" s="1">
-        <v>13500</v>
-      </c>
-      <c r="H36" s="1">
-        <v>5100</v>
-      </c>
-      <c r="I36" s="1">
-        <v>5100</v>
-      </c>
-      <c r="J36" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K36" s="1">
-        <v>1500</v>
+        <v>58</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -1630,33 +1614,68 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1">
         <v>6</v>
       </c>
       <c r="D37" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E37" s="1">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="F37" s="1">
         <v>6500</v>
       </c>
       <c r="G37" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H37" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I37" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F38" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G38" s="1">
         <v>14000</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H38" s="1">
         <v>5500</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I38" s="1">
         <v>5500</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J38" s="1">
         <v>2700</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K38" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 public stock ；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C50BE2B-19C0-4D17-80C6-032227159185}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964FE1B8-547C-4486-A33A-1033357DBAA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,14 @@
   </si>
   <si>
     <t>缴纳每块地产300元税金。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>证券中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得500元，然后额外获得你拥有投资项目数量*500元的奖励。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -593,11 +601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1190,39 +1198,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1">
-        <v>800</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1900</v>
-      </c>
-      <c r="F21" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G21" s="1">
-        <v>10500</v>
-      </c>
-      <c r="H21" s="1">
-        <v>4000</v>
-      </c>
-      <c r="I21" s="1">
-        <v>4000</v>
-      </c>
-      <c r="J21" s="1">
-        <v>2000</v>
-      </c>
-      <c r="K21" s="1">
-        <v>1200</v>
+        <v>60</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1230,7 +1214,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -1260,35 +1244,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>800</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G23" s="1">
+        <v>10500</v>
       </c>
       <c r="H23" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I23" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1296,34 +1304,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="1">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1">
-        <v>600</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F25" s="1">
-        <v>3500</v>
-      </c>
-      <c r="G25" s="1">
-        <v>7500</v>
-      </c>
-      <c r="H25" s="1">
-        <v>3000</v>
-      </c>
-      <c r="I25" s="1">
-        <v>3000</v>
-      </c>
-      <c r="J25" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K25" s="1">
-        <v>900</v>
+        <v>49</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1331,7 +1315,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -1340,22 +1324,22 @@
         <v>600</v>
       </c>
       <c r="E26" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G26" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H26" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J26" s="1">
         <v>1500</v>
-      </c>
-      <c r="F26" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G26" s="1">
-        <v>8500</v>
-      </c>
-      <c r="H26" s="1">
-        <v>3300</v>
-      </c>
-      <c r="I26" s="1">
-        <v>3300</v>
-      </c>
-      <c r="J26" s="1">
-        <v>1600</v>
       </c>
       <c r="K26" s="1">
         <v>900</v>
@@ -1366,10 +1350,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>600</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G27" s="1">
+        <v>8500</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3300</v>
+      </c>
+      <c r="I27" s="1">
+        <v>3300</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1600</v>
+      </c>
+      <c r="K27" s="1">
+        <v>900</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1377,89 +1385,65 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1">
-        <v>600</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F28" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G28" s="1">
-        <v>8000</v>
-      </c>
-      <c r="H28" s="1">
-        <v>3100</v>
-      </c>
-      <c r="I28" s="1">
-        <v>3100</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K28" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>600</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G29" s="1">
+        <v>8000</v>
       </c>
       <c r="H29" s="1">
-        <v>3500</v>
+        <v>3100</v>
       </c>
       <c r="I29" s="1">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="J29" s="1">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+      <c r="K29" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1">
-        <v>800</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F30" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G30" s="1">
-        <v>11000</v>
+        <v>36</v>
       </c>
       <c r="H30" s="1">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="I30" s="1">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="J30" s="1">
-        <v>2200</v>
-      </c>
-      <c r="K30" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1467,7 +1451,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1">
         <v>5</v>
@@ -1497,59 +1481,59 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>800</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G32" s="1">
+        <v>11000</v>
       </c>
       <c r="H32" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="I32" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="J32" s="1">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2200</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="1">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1">
-        <v>900</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2100</v>
-      </c>
-      <c r="F33" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G33" s="1">
-        <v>12000</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="I33" s="1">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="J33" s="1">
-        <v>2400</v>
-      </c>
-      <c r="K33" s="1">
-        <v>1200</v>
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -1557,10 +1541,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1">
+        <v>900</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G34" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2400</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -1568,34 +1576,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E35" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F35" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G35" s="1">
-        <v>13000</v>
-      </c>
-      <c r="H35" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I35" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J35" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K35" s="1">
-        <v>1500</v>
+        <v>55</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -1603,10 +1587,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F36" s="1">
+        <v>6000</v>
+      </c>
+      <c r="G36" s="1">
+        <v>13000</v>
+      </c>
+      <c r="H36" s="1">
+        <v>5000</v>
+      </c>
+      <c r="I36" s="1">
+        <v>5000</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -1614,34 +1622,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="1">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E37" s="1">
-        <v>2400</v>
-      </c>
-      <c r="F37" s="1">
-        <v>6500</v>
-      </c>
-      <c r="G37" s="1">
-        <v>13500</v>
-      </c>
-      <c r="H37" s="1">
-        <v>5100</v>
-      </c>
-      <c r="I37" s="1">
-        <v>5100</v>
-      </c>
-      <c r="J37" s="1">
-        <v>2500</v>
-      </c>
-      <c r="K37" s="1">
-        <v>1500</v>
+        <v>58</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -1649,33 +1633,68 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1">
         <v>6</v>
       </c>
       <c r="D38" s="1">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="E38" s="1">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="F38" s="1">
         <v>6500</v>
       </c>
       <c r="G38" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H38" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I38" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J38" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="1">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F39" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G39" s="1">
         <v>14000</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H39" s="1">
         <v>5500</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I39" s="1">
         <v>5500</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J39" s="1">
         <v>2700</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K39" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
完成 public goto prison ；
</commit_message>
<xml_diff>
--- a/doc/test/map_test.xlsx
+++ b/doc/test/map_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964FE1B8-547C-4486-A33A-1033357DBAA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F3979-4A10-4C42-8575-1CD014FFC00A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,6 +267,22 @@
   </si>
   <si>
     <t>获得500元，然后额外获得你拥有投资项目数量*500元的奖励。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>监狱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停留一回合。当你在监狱时，不能收取租金或获得任何金钱奖励。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入狱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立即进入监狱并停留一回合。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -601,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -937,39 +953,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>300</v>
-      </c>
-      <c r="E12" s="1">
-        <v>700</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1500</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3500</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1800</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1800</v>
-      </c>
-      <c r="J12" s="1">
-        <v>900</v>
-      </c>
-      <c r="K12" s="1">
-        <v>300</v>
+        <v>62</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -977,89 +969,89 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E13" s="1">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="F13" s="1">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="G13" s="1">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="H13" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="I13" s="1">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="J13" s="1">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="K13" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>400</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5500</v>
       </c>
       <c r="H14" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="I14" s="1">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+      <c r="K14" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>400</v>
-      </c>
-      <c r="E15" s="1">
-        <v>900</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G15" s="1">
-        <v>5000</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I15" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J15" s="1">
-        <v>1000</v>
-      </c>
-      <c r="K15" s="1">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1067,10 +1059,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>400</v>
+      </c>
+      <c r="E16" s="1">
+        <v>900</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K16" s="1">
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1078,89 +1094,65 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>400</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G17" s="1">
-        <v>5500</v>
-      </c>
-      <c r="H17" s="1">
-        <v>2200</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2200</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1100</v>
-      </c>
-      <c r="K17" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>400</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G18" s="1">
+        <v>5500</v>
       </c>
       <c r="H18" s="1">
-        <v>3500</v>
+        <v>2200</v>
       </c>
       <c r="I18" s="1">
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+      <c r="K18" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1">
-        <v>700</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1600</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4500</v>
-      </c>
-      <c r="G19" s="1">
-        <v>9000</v>
+        <v>51</v>
       </c>
       <c r="H19" s="1">
-        <v>3800</v>
+        <v>3500</v>
       </c>
       <c r="I19" s="1">
-        <v>3800</v>
+        <v>3000</v>
       </c>
       <c r="J19" s="1">
-        <v>1900</v>
-      </c>
-      <c r="K19" s="1">
-        <v>900</v>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1168,7 +1160,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1177,71 +1169,71 @@
         <v>700</v>
       </c>
       <c r="E20" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="F20" s="1">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="G20" s="1">
-        <v>8500</v>
+        <v>9000</v>
       </c>
       <c r="H20" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="I20" s="1">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="J20" s="1">
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="K20" s="1">
         <v>900</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>700</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G21" s="1">
+        <v>8500</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3500</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3500</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1700</v>
+      </c>
+      <c r="K21" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3</v>
-      </c>
-      <c r="D22" s="1">
-        <v>800</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1900</v>
-      </c>
-      <c r="F22" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G22" s="1">
-        <v>10500</v>
-      </c>
-      <c r="H22" s="1">
-        <v>4000</v>
-      </c>
-      <c r="I22" s="1">
-        <v>4000</v>
-      </c>
-      <c r="J22" s="1">
-        <v>2000</v>
-      </c>
-      <c r="K22" s="1">
-        <v>1200</v>
+        <v>60</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1249,7 +1241,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -1279,24 +1271,39 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>800</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G24" s="1">
+        <v>10500</v>
       </c>
       <c r="H24" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="I24" s="1">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>31</v>
+        <v>2000</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1304,33 +1311,18 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="1">
-        <v>4</v>
-      </c>
-      <c r="D26" s="1">
-        <v>600</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1400</v>
-      </c>
-      <c r="F26" s="1">
-        <v>3500</v>
-      </c>
-      <c r="G26" s="1">
-        <v>7500</v>
+        <v>32</v>
       </c>
       <c r="H26" s="1">
         <v>3000</v>
@@ -1339,10 +1331,10 @@
         <v>3000</v>
       </c>
       <c r="J26" s="1">
-        <v>1500</v>
-      </c>
-      <c r="K26" s="1">
-        <v>900</v>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1350,34 +1342,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" s="1">
-        <v>600</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1500</v>
-      </c>
-      <c r="F27" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G27" s="1">
-        <v>8500</v>
-      </c>
-      <c r="H27" s="1">
-        <v>3300</v>
-      </c>
-      <c r="I27" s="1">
-        <v>3300</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1600</v>
-      </c>
-      <c r="K27" s="1">
-        <v>900</v>
+        <v>49</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1385,10 +1353,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>57</v>
+        <v>33</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>600</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G28" s="1">
+        <v>7500</v>
+      </c>
+      <c r="H28" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1500</v>
+      </c>
+      <c r="K28" s="1">
+        <v>900</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1396,54 +1388,45 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <v>600</v>
       </c>
       <c r="E29" s="1">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="F29" s="1">
         <v>4000</v>
       </c>
       <c r="G29" s="1">
-        <v>8000</v>
+        <v>8500</v>
       </c>
       <c r="H29" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="I29" s="1">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="J29" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="K29" s="1">
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="1">
-        <v>3500</v>
-      </c>
-      <c r="I30" s="1">
-        <v>3000</v>
-      </c>
-      <c r="J30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1451,89 +1434,89 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
         <v>5</v>
       </c>
       <c r="D31" s="1">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E31" s="1">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="F31" s="1">
-        <v>5500</v>
+        <v>4000</v>
       </c>
       <c r="G31" s="1">
-        <v>11000</v>
+        <v>8000</v>
       </c>
       <c r="H31" s="1">
-        <v>4400</v>
+        <v>3100</v>
       </c>
       <c r="I31" s="1">
-        <v>4400</v>
+        <v>3100</v>
       </c>
       <c r="J31" s="1">
-        <v>2200</v>
+        <v>1500</v>
       </c>
       <c r="K31" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="1">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1">
-        <v>800</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F32" s="1">
-        <v>5500</v>
-      </c>
-      <c r="G32" s="1">
-        <v>11000</v>
+        <v>36</v>
       </c>
       <c r="H32" s="1">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="I32" s="1">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="J32" s="1">
-        <v>2200</v>
-      </c>
-      <c r="K32" s="1">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C33" s="1">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>800</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G33" s="1">
+        <v>11000</v>
       </c>
       <c r="H33" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="I33" s="1">
-        <v>3000</v>
+        <v>4400</v>
       </c>
       <c r="J33" s="1">
-        <v>0</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>31</v>
+        <v>2200</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -1541,45 +1524,54 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="E34" s="1">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="F34" s="1">
         <v>5500</v>
       </c>
       <c r="G34" s="1">
-        <v>12000</v>
+        <v>11000</v>
       </c>
       <c r="H34" s="1">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="I34" s="1">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="J34" s="1">
-        <v>2400</v>
+        <v>2200</v>
       </c>
       <c r="K34" s="1">
         <v>1200</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
+      </c>
+      <c r="H35" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -1587,34 +1579,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
       </c>
       <c r="D36" s="1">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="E36" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F36" s="1">
+        <v>5500</v>
+      </c>
+      <c r="G36" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I36" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J36" s="1">
         <v>2400</v>
       </c>
-      <c r="F36" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G36" s="1">
-        <v>13000</v>
-      </c>
-      <c r="H36" s="1">
-        <v>5000</v>
-      </c>
-      <c r="I36" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J36" s="1">
-        <v>2500</v>
-      </c>
       <c r="K36" s="1">
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -1622,10 +1614,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -1633,7 +1625,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1">
         <v>6</v>
@@ -1645,16 +1637,16 @@
         <v>2400</v>
       </c>
       <c r="F38" s="1">
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="G38" s="1">
-        <v>13500</v>
+        <v>13000</v>
       </c>
       <c r="H38" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="I38" s="1">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="J38" s="1">
         <v>2500</v>
@@ -1668,33 +1660,79 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6500</v>
+      </c>
+      <c r="G40" s="1">
+        <v>13500</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5100</v>
+      </c>
+      <c r="I40" s="1">
+        <v>5100</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2500</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C41" s="1">
         <v>6</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D41" s="1">
         <v>1100</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E41" s="1">
         <v>2500</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F41" s="1">
         <v>6500</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G41" s="1">
         <v>14000</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H41" s="1">
         <v>5500</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I41" s="1">
         <v>5500</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J41" s="1">
         <v>2700</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K41" s="1">
         <v>1500</v>
       </c>
     </row>

</xml_diff>